<commit_message>
buffers adicionados a classificação dos solos
</commit_message>
<xml_diff>
--- a/cos/longtable_com_soloescrito.xlsx
+++ b/cos/longtable_com_soloescrito.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H49"/>
+  <dimension ref="A1:I49"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -465,10 +465,15 @@
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
+          <t>Uso_solo_simplificado</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
           <t>Urbanizado</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>Transporte</t>
         </is>
@@ -495,10 +500,15 @@
       <c r="F2" t="n">
         <v>20.64603079546817</v>
       </c>
-      <c r="G2" t="n">
-        <v>0</v>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H2" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" t="n">
         <v>0</v>
       </c>
     </row>
@@ -523,10 +533,15 @@
       <c r="F3" t="n">
         <v>32.93764130559803</v>
       </c>
-      <c r="G3" t="n">
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>Urbanizado</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
         <v>1</v>
       </c>
-      <c r="H3" t="n">
+      <c r="I3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -551,10 +566,15 @@
       <c r="F4" t="n">
         <v>18.85869837746607</v>
       </c>
-      <c r="G4" t="n">
-        <v>0</v>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H4" t="n">
+        <v>0</v>
+      </c>
+      <c r="I4" t="n">
         <v>0</v>
       </c>
     </row>
@@ -579,10 +599,15 @@
       <c r="F5" t="n">
         <v>32.89084930364226</v>
       </c>
-      <c r="G5" t="n">
-        <v>0</v>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>Transporte</t>
+        </is>
       </c>
       <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="I5" t="n">
         <v>1</v>
       </c>
     </row>
@@ -607,10 +632,15 @@
       <c r="F6" t="n">
         <v>21.89124717822572</v>
       </c>
-      <c r="G6" t="n">
-        <v>0</v>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H6" t="n">
+        <v>0</v>
+      </c>
+      <c r="I6" t="n">
         <v>0</v>
       </c>
     </row>
@@ -635,10 +665,15 @@
       <c r="F7" t="n">
         <v>18.73569299496276</v>
       </c>
-      <c r="G7" t="n">
-        <v>0</v>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H7" t="n">
+        <v>0</v>
+      </c>
+      <c r="I7" t="n">
         <v>0</v>
       </c>
     </row>
@@ -663,10 +698,15 @@
       <c r="F8" t="n">
         <v>28.20358804427715</v>
       </c>
-      <c r="G8" t="n">
-        <v>0</v>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H8" t="n">
+        <v>0</v>
+      </c>
+      <c r="I8" t="n">
         <v>0</v>
       </c>
     </row>
@@ -691,10 +731,15 @@
       <c r="F9" t="n">
         <v>16.79738220759935</v>
       </c>
-      <c r="G9" t="n">
-        <v>0</v>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H9" t="n">
+        <v>0</v>
+      </c>
+      <c r="I9" t="n">
         <v>0</v>
       </c>
     </row>
@@ -719,10 +764,15 @@
       <c r="F10" t="n">
         <v>23.06041636353474</v>
       </c>
-      <c r="G10" t="n">
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>Urbanizado</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
         <v>1</v>
       </c>
-      <c r="H10" t="n">
+      <c r="I10" t="n">
         <v>0</v>
       </c>
     </row>
@@ -747,10 +797,15 @@
       <c r="F11" t="n">
         <v>24.21703155113064</v>
       </c>
-      <c r="G11" t="n">
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>Urbanizado</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
         <v>1</v>
       </c>
-      <c r="H11" t="n">
+      <c r="I11" t="n">
         <v>0</v>
       </c>
     </row>
@@ -775,10 +830,15 @@
       <c r="F12" t="n">
         <v>15.45705537044591</v>
       </c>
-      <c r="G12" t="n">
-        <v>0</v>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H12" t="n">
+        <v>0</v>
+      </c>
+      <c r="I12" t="n">
         <v>0</v>
       </c>
     </row>
@@ -803,10 +863,15 @@
       <c r="F13" t="n">
         <v>29.74194464589739</v>
       </c>
-      <c r="G13" t="n">
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>Urbanizado</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
         <v>1</v>
       </c>
-      <c r="H13" t="n">
+      <c r="I13" t="n">
         <v>0</v>
       </c>
     </row>
@@ -831,10 +896,15 @@
       <c r="F14" t="n">
         <v>9.911897496874564</v>
       </c>
-      <c r="G14" t="n">
-        <v>0</v>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H14" t="n">
+        <v>0</v>
+      </c>
+      <c r="I14" t="n">
         <v>0</v>
       </c>
     </row>
@@ -859,10 +929,15 @@
       <c r="F15" t="n">
         <v>31.7736527854409</v>
       </c>
-      <c r="G15" t="n">
-        <v>0</v>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Transporte</t>
+        </is>
       </c>
       <c r="H15" t="n">
+        <v>0</v>
+      </c>
+      <c r="I15" t="n">
         <v>1</v>
       </c>
     </row>
@@ -887,10 +962,15 @@
       <c r="F16" t="n">
         <v>22.68205445900004</v>
       </c>
-      <c r="G16" t="n">
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>Urbanizado</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
         <v>1</v>
       </c>
-      <c r="H16" t="n">
+      <c r="I16" t="n">
         <v>0</v>
       </c>
     </row>
@@ -915,10 +995,15 @@
       <c r="F17" t="n">
         <v>25.17787668475592</v>
       </c>
-      <c r="G17" t="n">
-        <v>0</v>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H17" t="n">
+        <v>0</v>
+      </c>
+      <c r="I17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -943,10 +1028,15 @@
       <c r="F18" t="n">
         <v>33.82417065389357</v>
       </c>
-      <c r="G18" t="n">
-        <v>0</v>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H18" t="n">
+        <v>0</v>
+      </c>
+      <c r="I18" t="n">
         <v>0</v>
       </c>
     </row>
@@ -971,10 +1061,15 @@
       <c r="F19" t="n">
         <v>18.94870887804427</v>
       </c>
-      <c r="G19" t="n">
-        <v>0</v>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H19" t="n">
+        <v>0</v>
+      </c>
+      <c r="I19" t="n">
         <v>0</v>
       </c>
     </row>
@@ -999,10 +1094,15 @@
       <c r="F20" t="n">
         <v>28.03150538351018</v>
       </c>
-      <c r="G20" t="n">
-        <v>0</v>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H20" t="n">
+        <v>0</v>
+      </c>
+      <c r="I20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1027,10 +1127,15 @@
       <c r="F21" t="n">
         <v>14.67341021479265</v>
       </c>
-      <c r="G21" t="n">
-        <v>0</v>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H21" t="n">
+        <v>0</v>
+      </c>
+      <c r="I21" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1055,10 +1160,15 @@
       <c r="F22" t="n">
         <v>23.03242851249266</v>
       </c>
-      <c r="G22" t="n">
-        <v>0</v>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>Transporte</t>
+        </is>
       </c>
       <c r="H22" t="n">
+        <v>0</v>
+      </c>
+      <c r="I22" t="n">
         <v>1</v>
       </c>
     </row>
@@ -1083,10 +1193,15 @@
       <c r="F23" t="n">
         <v>15.10060868609654</v>
       </c>
-      <c r="G23" t="n">
-        <v>0</v>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H23" t="n">
+        <v>0</v>
+      </c>
+      <c r="I23" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1111,10 +1226,15 @@
       <c r="F24" t="n">
         <v>14.6387783591567</v>
       </c>
-      <c r="G24" t="n">
-        <v>0</v>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H24" t="n">
+        <v>0</v>
+      </c>
+      <c r="I24" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1139,10 +1259,15 @@
       <c r="F25" t="n">
         <v>18.55732009616839</v>
       </c>
-      <c r="G25" t="n">
-        <v>0</v>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H25" t="n">
+        <v>0</v>
+      </c>
+      <c r="I25" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1167,10 +1292,15 @@
       <c r="F26" t="n">
         <v>24.40424949410358</v>
       </c>
-      <c r="G26" t="n">
-        <v>0</v>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H26" t="n">
+        <v>0</v>
+      </c>
+      <c r="I26" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1195,10 +1325,15 @@
       <c r="F27" t="n">
         <v>23.26173016194345</v>
       </c>
-      <c r="G27" t="n">
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>Urbanizado</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
         <v>1</v>
       </c>
-      <c r="H27" t="n">
+      <c r="I27" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1223,10 +1358,15 @@
       <c r="F28" t="n">
         <v>27.02458913103547</v>
       </c>
-      <c r="G28" t="n">
-        <v>0</v>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H28" t="n">
+        <v>0</v>
+      </c>
+      <c r="I28" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1251,10 +1391,15 @@
       <c r="F29" t="n">
         <v>32.97233577505904</v>
       </c>
-      <c r="G29" t="n">
-        <v>0</v>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="I29" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1279,10 +1424,15 @@
       <c r="F30" t="n">
         <v>33.6246065931518</v>
       </c>
-      <c r="G30" t="n">
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Urbanizado</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
         <v>1</v>
       </c>
-      <c r="H30" t="n">
+      <c r="I30" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1307,10 +1457,15 @@
       <c r="F31" t="n">
         <v>27.97678762543504</v>
       </c>
-      <c r="G31" t="n">
-        <v>0</v>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H31" t="n">
+        <v>0</v>
+      </c>
+      <c r="I31" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1335,10 +1490,15 @@
       <c r="F32" t="n">
         <v>25.45935860930451</v>
       </c>
-      <c r="G32" t="n">
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>Urbanizado</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
         <v>1</v>
       </c>
-      <c r="H32" t="n">
+      <c r="I32" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1363,10 +1523,15 @@
       <c r="F33" t="n">
         <v>29.89094651229147</v>
       </c>
-      <c r="G33" t="n">
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Urbanizado</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
         <v>1</v>
       </c>
-      <c r="H33" t="n">
+      <c r="I33" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1391,10 +1556,15 @@
       <c r="F34" t="n">
         <v>22.66369613285387</v>
       </c>
-      <c r="G34" t="n">
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>Urbanizado</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
         <v>1</v>
       </c>
-      <c r="H34" t="n">
+      <c r="I34" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1419,10 +1589,15 @@
       <c r="F35" t="n">
         <v>26.55954726445246</v>
       </c>
-      <c r="G35" t="n">
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>Urbanizado</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
         <v>1</v>
       </c>
-      <c r="H35" t="n">
+      <c r="I35" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1447,10 +1622,15 @@
       <c r="F36" t="n">
         <v>21.24585750058139</v>
       </c>
-      <c r="G36" t="n">
-        <v>0</v>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H36" t="n">
+        <v>0</v>
+      </c>
+      <c r="I36" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1475,10 +1655,15 @@
       <c r="F37" t="n">
         <v>25.25524961832934</v>
       </c>
-      <c r="G37" t="n">
-        <v>0</v>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H37" t="n">
+        <v>0</v>
+      </c>
+      <c r="I37" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1503,10 +1688,15 @@
       <c r="F38" t="n">
         <v>28.63738323879013</v>
       </c>
-      <c r="G38" t="n">
-        <v>0</v>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="I38" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1531,10 +1721,15 @@
       <c r="F39" t="n">
         <v>31.03275876896798</v>
       </c>
-      <c r="G39" t="n">
-        <v>0</v>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H39" t="n">
+        <v>0</v>
+      </c>
+      <c r="I39" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1559,10 +1754,15 @@
       <c r="F40" t="n">
         <v>18.62189344545493</v>
       </c>
-      <c r="G40" t="n">
-        <v>0</v>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H40" t="n">
+        <v>0</v>
+      </c>
+      <c r="I40" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1587,10 +1787,15 @@
       <c r="F41" t="n">
         <v>33.57066858262246</v>
       </c>
-      <c r="G41" t="n">
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>Urbanizado</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
         <v>1</v>
       </c>
-      <c r="H41" t="n">
+      <c r="I41" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1615,10 +1820,15 @@
       <c r="F42" t="n">
         <v>18.08886559205197</v>
       </c>
-      <c r="G42" t="n">
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Urbanizado</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
         <v>1</v>
       </c>
-      <c r="H42" t="n">
+      <c r="I42" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1643,10 +1853,15 @@
       <c r="F43" t="n">
         <v>33.01948570155671</v>
       </c>
-      <c r="G43" t="n">
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>Urbanizado</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
         <v>1</v>
       </c>
-      <c r="H43" t="n">
+      <c r="I43" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1671,10 +1886,15 @@
       <c r="F44" t="n">
         <v>29.65253984794291</v>
       </c>
-      <c r="G44" t="n">
-        <v>0</v>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H44" t="n">
+        <v>0</v>
+      </c>
+      <c r="I44" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1699,10 +1919,15 @@
       <c r="F45" t="n">
         <v>29.48644693160862</v>
       </c>
-      <c r="G45" t="n">
-        <v>0</v>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H45" t="n">
+        <v>0</v>
+      </c>
+      <c r="I45" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1727,10 +1952,15 @@
       <c r="F46" t="n">
         <v>23.30881037668967</v>
       </c>
-      <c r="G46" t="n">
-        <v>0</v>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H46" t="n">
+        <v>0</v>
+      </c>
+      <c r="I46" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1755,10 +1985,15 @@
       <c r="F47" t="n">
         <v>24.91582792010203</v>
       </c>
-      <c r="G47" t="n">
-        <v>0</v>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H47" t="n">
+        <v>0</v>
+      </c>
+      <c r="I47" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1783,10 +2018,15 @@
       <c r="F48" t="n">
         <v>22.57544372407552</v>
       </c>
-      <c r="G48" t="n">
-        <v>0</v>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H48" t="n">
+        <v>0</v>
+      </c>
+      <c r="I48" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1811,10 +2051,15 @@
       <c r="F49" t="n">
         <v>22.30368022065842</v>
       </c>
-      <c r="G49" t="n">
-        <v>0</v>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>Outros</t>
+        </is>
       </c>
       <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="I49" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>